<commit_message>
Tag 3 - Backup Commit und Push
</commit_message>
<xml_diff>
--- a/ipa zeitplan.xlsx
+++ b/ipa zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\IdeaProjects\IPA_2024_Docs\IPA_2024_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D99221-341E-4F27-B448-F903CA719EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED620277-D24C-4464-BDF5-3C1B23EB0847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DAB00B04-B062-47DB-8ACF-D401D96AFC5E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Zeitplan - IPA</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Teil 1 - Administrativer Teil</t>
+  </si>
+  <si>
+    <t>1,5</t>
   </si>
 </sst>
 </file>
@@ -659,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1138,6 +1141,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
@@ -1475,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF7E634-E7D3-4035-B3D3-3551A9582348}">
   <dimension ref="A1:BS625"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE36" sqref="AE36"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AJ31" sqref="AJ31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,7 +2061,9 @@
       <c r="AB7" s="25"/>
       <c r="AC7" s="24"/>
       <c r="AD7" s="24"/>
-      <c r="AE7" s="24"/>
+      <c r="AE7" s="149">
+        <v>1</v>
+      </c>
       <c r="AF7" s="25"/>
       <c r="AG7" s="24"/>
       <c r="AH7" s="24"/>
@@ -3004,7 +3015,9 @@
       </c>
       <c r="P20" s="45"/>
       <c r="Q20" s="46"/>
-      <c r="R20" s="44"/>
+      <c r="R20" s="44">
+        <v>0.5</v>
+      </c>
       <c r="S20" s="45"/>
       <c r="T20" s="46"/>
       <c r="U20" s="8"/>
@@ -3086,7 +3099,9 @@
       <c r="AA21" s="7"/>
       <c r="AB21" s="16"/>
       <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
+      <c r="AD21" s="40">
+        <v>0.5</v>
+      </c>
       <c r="AE21" s="7"/>
       <c r="AF21" s="16"/>
       <c r="AG21" s="7"/>
@@ -3146,7 +3161,9 @@
       </c>
       <c r="P22" s="45"/>
       <c r="Q22" s="46"/>
-      <c r="R22" s="44"/>
+      <c r="R22" s="44">
+        <v>1.5</v>
+      </c>
       <c r="S22" s="45"/>
       <c r="T22" s="46"/>
       <c r="U22" s="8"/>
@@ -3227,7 +3244,9 @@
       <c r="Z23" s="24"/>
       <c r="AA23" s="24"/>
       <c r="AB23" s="25"/>
-      <c r="AC23" s="24"/>
+      <c r="AC23" s="149">
+        <v>1.5</v>
+      </c>
       <c r="AD23" s="24"/>
       <c r="AE23" s="24"/>
       <c r="AF23" s="25"/>
@@ -3290,7 +3309,9 @@
       </c>
       <c r="P24" s="45"/>
       <c r="Q24" s="46"/>
-      <c r="R24" s="44"/>
+      <c r="R24" s="44">
+        <v>0.5</v>
+      </c>
       <c r="S24" s="45"/>
       <c r="T24" s="46"/>
       <c r="U24" s="8"/>
@@ -3375,8 +3396,10 @@
       <c r="AB25" s="25"/>
       <c r="AC25" s="24"/>
       <c r="AD25" s="24"/>
-      <c r="AE25" s="24"/>
-      <c r="AF25" s="25"/>
+      <c r="AE25" s="149">
+        <v>0.5</v>
+      </c>
+      <c r="AF25" s="163"/>
       <c r="AG25" s="24"/>
       <c r="AH25" s="24"/>
       <c r="AI25" s="24"/>
@@ -5257,7 +5280,7 @@
       <c r="AB51" s="16"/>
       <c r="AC51" s="7"/>
       <c r="AD51" s="7"/>
-      <c r="AE51" s="7"/>
+      <c r="AE51" s="162"/>
       <c r="AF51" s="16"/>
       <c r="AG51" s="7"/>
       <c r="AH51" s="7"/>
@@ -5471,7 +5494,7 @@
       <c r="P54" s="45"/>
       <c r="Q54" s="46"/>
       <c r="R54" s="44">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="S54" s="45"/>
       <c r="T54" s="46"/>
@@ -5559,10 +5582,18 @@
       <c r="AB55" s="38">
         <v>1.5</v>
       </c>
-      <c r="AC55" s="7"/>
-      <c r="AD55" s="7"/>
-      <c r="AE55" s="7"/>
-      <c r="AF55" s="16"/>
+      <c r="AC55" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="AD55" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE55" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="AF55" s="38">
+        <v>0.5</v>
+      </c>
       <c r="AG55" s="7"/>
       <c r="AH55" s="7"/>
       <c r="AI55" s="7"/>
@@ -5620,7 +5651,9 @@
       </c>
       <c r="P56" s="45"/>
       <c r="Q56" s="46"/>
-      <c r="R56" s="44"/>
+      <c r="R56" s="44">
+        <v>1</v>
+      </c>
       <c r="S56" s="45"/>
       <c r="T56" s="46"/>
       <c r="U56" s="8"/>
@@ -5704,7 +5737,9 @@
       <c r="AC57" s="23"/>
       <c r="AD57" s="7"/>
       <c r="AE57" s="7"/>
-      <c r="AF57" s="16"/>
+      <c r="AF57" s="38">
+        <v>1</v>
+      </c>
       <c r="AG57" s="7"/>
       <c r="AH57" s="7"/>
       <c r="AI57" s="7"/>
@@ -6308,7 +6343,9 @@
       <c r="AC65" s="7"/>
       <c r="AD65" s="7"/>
       <c r="AE65" s="7"/>
-      <c r="AF65" s="16"/>
+      <c r="AF65" s="38">
+        <v>0.5</v>
+      </c>
       <c r="AG65" s="7"/>
       <c r="AH65" s="7"/>
       <c r="AI65" s="7"/>
@@ -6659,7 +6696,7 @@
       <c r="Q70" s="71"/>
       <c r="R70" s="66">
         <f>SUM(R6:T69)</f>
-        <v>16</v>
+        <v>22.5</v>
       </c>
       <c r="S70" s="67"/>
       <c r="T70" s="68"/>
@@ -6674,11 +6711,15 @@
       <c r="Y70" s="62"/>
       <c r="Z70" s="62"/>
       <c r="AA70" s="62"/>
-      <c r="AB70" s="13"/>
+      <c r="AB70" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="AC70" s="62"/>
       <c r="AD70" s="62"/>
       <c r="AE70" s="62"/>
-      <c r="AF70" s="13"/>
+      <c r="AF70" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="AG70" s="62"/>
       <c r="AH70" s="62"/>
       <c r="AI70" s="62"/>

</xml_diff>

<commit_message>
Tag 5 - Backup Commit und Push
</commit_message>
<xml_diff>
--- a/ipa zeitplan.xlsx
+++ b/ipa zeitplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\IdeaProjects\IPA_2024_Docs\IPA_2024_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE8B369-D8AE-42A3-875D-6C0FF366605E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966DBEC8-E240-41CB-94CE-FF0DA330C6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DAB00B04-B062-47DB-8ACF-D401D96AFC5E}"/>
   </bookViews>
@@ -662,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -870,6 +870,60 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -879,38 +933,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -924,12 +954,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -948,15 +972,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -969,21 +984,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1124,6 +1124,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1462,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF7E634-E7D3-4035-B3D3-3551A9582348}">
   <dimension ref="A1:BN625"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG36" sqref="AG36"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,50 +1500,50 @@
       <c r="R1" s="128"/>
       <c r="S1" s="128"/>
       <c r="T1" s="128"/>
-      <c r="U1" s="106"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="106"/>
-      <c r="X1" s="106"/>
-      <c r="Y1" s="106"/>
-      <c r="Z1" s="106"/>
-      <c r="AA1" s="106"/>
-      <c r="AB1" s="106"/>
-      <c r="AC1" s="106"/>
-      <c r="AD1" s="106"/>
-      <c r="AE1" s="106"/>
-      <c r="AF1" s="106"/>
-      <c r="AG1" s="106"/>
-      <c r="AH1" s="106"/>
-      <c r="AI1" s="106"/>
-      <c r="AJ1" s="106"/>
-      <c r="AK1" s="106"/>
-      <c r="AL1" s="106"/>
-      <c r="AM1" s="106"/>
-      <c r="AN1" s="106"/>
-      <c r="AO1" s="106"/>
-      <c r="AP1" s="106"/>
-      <c r="AQ1" s="106"/>
-      <c r="AR1" s="106"/>
-      <c r="AS1" s="106"/>
-      <c r="AT1" s="106"/>
-      <c r="AU1" s="106"/>
-      <c r="AV1" s="106"/>
-      <c r="AW1" s="106"/>
-      <c r="AX1" s="106"/>
-      <c r="AY1" s="106"/>
-      <c r="AZ1" s="106"/>
-      <c r="BA1" s="106"/>
-      <c r="BB1" s="106"/>
-      <c r="BC1" s="106"/>
-      <c r="BD1" s="106"/>
-      <c r="BE1" s="106"/>
-      <c r="BF1" s="106"/>
-      <c r="BG1" s="106"/>
-      <c r="BH1" s="106"/>
-      <c r="BI1" s="106"/>
-      <c r="BJ1" s="106"/>
-      <c r="BK1" s="106"/>
-      <c r="BL1" s="106"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="92"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="92"/>
+      <c r="AI1" s="92"/>
+      <c r="AJ1" s="92"/>
+      <c r="AK1" s="92"/>
+      <c r="AL1" s="92"/>
+      <c r="AM1" s="92"/>
+      <c r="AN1" s="92"/>
+      <c r="AO1" s="92"/>
+      <c r="AP1" s="92"/>
+      <c r="AQ1" s="92"/>
+      <c r="AR1" s="92"/>
+      <c r="AS1" s="92"/>
+      <c r="AT1" s="92"/>
+      <c r="AU1" s="92"/>
+      <c r="AV1" s="92"/>
+      <c r="AW1" s="92"/>
+      <c r="AX1" s="92"/>
+      <c r="AY1" s="92"/>
+      <c r="AZ1" s="92"/>
+      <c r="BA1" s="92"/>
+      <c r="BB1" s="92"/>
+      <c r="BC1" s="92"/>
+      <c r="BD1" s="92"/>
+      <c r="BE1" s="92"/>
+      <c r="BF1" s="92"/>
+      <c r="BG1" s="92"/>
+      <c r="BH1" s="92"/>
+      <c r="BI1" s="92"/>
+      <c r="BJ1" s="92"/>
+      <c r="BK1" s="92"/>
+      <c r="BL1" s="92"/>
       <c r="BM1" s="43"/>
     </row>
     <row r="2" spans="1:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1574,21 +1580,21 @@
       <c r="AE2" s="42"/>
       <c r="AF2" s="42"/>
       <c r="AG2" s="6"/>
-      <c r="AH2" s="108" t="s">
+      <c r="AH2" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="AI2" s="108"/>
-      <c r="AJ2" s="108"/>
-      <c r="AK2" s="108"/>
-      <c r="AL2" s="108"/>
+      <c r="AI2" s="94"/>
+      <c r="AJ2" s="94"/>
+      <c r="AK2" s="94"/>
+      <c r="AL2" s="94"/>
       <c r="AM2" s="9"/>
-      <c r="AN2" s="108" t="s">
+      <c r="AN2" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="AO2" s="108"/>
-      <c r="AP2" s="108"/>
-      <c r="AQ2" s="108"/>
-      <c r="AR2" s="108"/>
+      <c r="AO2" s="94"/>
+      <c r="AP2" s="94"/>
+      <c r="AQ2" s="94"/>
+      <c r="AR2" s="94"/>
       <c r="AS2" s="142"/>
       <c r="AT2" s="142"/>
       <c r="AU2" s="142"/>
@@ -1632,50 +1638,50 @@
       <c r="R3" s="130"/>
       <c r="S3" s="130"/>
       <c r="T3" s="130"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-      <c r="X3" s="107"/>
-      <c r="Y3" s="107"/>
-      <c r="Z3" s="107"/>
-      <c r="AA3" s="107"/>
-      <c r="AB3" s="107"/>
-      <c r="AC3" s="107"/>
-      <c r="AD3" s="107"/>
-      <c r="AE3" s="107"/>
-      <c r="AF3" s="107"/>
-      <c r="AG3" s="107"/>
-      <c r="AH3" s="107"/>
-      <c r="AI3" s="107"/>
-      <c r="AJ3" s="107"/>
-      <c r="AK3" s="107"/>
-      <c r="AL3" s="107"/>
-      <c r="AM3" s="107"/>
-      <c r="AN3" s="107"/>
-      <c r="AO3" s="107"/>
-      <c r="AP3" s="107"/>
-      <c r="AQ3" s="107"/>
-      <c r="AR3" s="107"/>
-      <c r="AS3" s="107"/>
-      <c r="AT3" s="107"/>
-      <c r="AU3" s="107"/>
-      <c r="AV3" s="107"/>
-      <c r="AW3" s="107"/>
-      <c r="AX3" s="107"/>
-      <c r="AY3" s="107"/>
-      <c r="AZ3" s="107"/>
-      <c r="BA3" s="107"/>
-      <c r="BB3" s="107"/>
-      <c r="BC3" s="107"/>
-      <c r="BD3" s="107"/>
-      <c r="BE3" s="107"/>
-      <c r="BF3" s="107"/>
-      <c r="BG3" s="107"/>
-      <c r="BH3" s="107"/>
-      <c r="BI3" s="107"/>
-      <c r="BJ3" s="107"/>
-      <c r="BK3" s="107"/>
-      <c r="BL3" s="107"/>
+      <c r="U3" s="93"/>
+      <c r="V3" s="93"/>
+      <c r="W3" s="93"/>
+      <c r="X3" s="93"/>
+      <c r="Y3" s="93"/>
+      <c r="Z3" s="93"/>
+      <c r="AA3" s="93"/>
+      <c r="AB3" s="93"/>
+      <c r="AC3" s="93"/>
+      <c r="AD3" s="93"/>
+      <c r="AE3" s="93"/>
+      <c r="AF3" s="93"/>
+      <c r="AG3" s="93"/>
+      <c r="AH3" s="93"/>
+      <c r="AI3" s="93"/>
+      <c r="AJ3" s="93"/>
+      <c r="AK3" s="93"/>
+      <c r="AL3" s="93"/>
+      <c r="AM3" s="93"/>
+      <c r="AN3" s="93"/>
+      <c r="AO3" s="93"/>
+      <c r="AP3" s="93"/>
+      <c r="AQ3" s="93"/>
+      <c r="AR3" s="93"/>
+      <c r="AS3" s="93"/>
+      <c r="AT3" s="93"/>
+      <c r="AU3" s="93"/>
+      <c r="AV3" s="93"/>
+      <c r="AW3" s="93"/>
+      <c r="AX3" s="93"/>
+      <c r="AY3" s="93"/>
+      <c r="AZ3" s="93"/>
+      <c r="BA3" s="93"/>
+      <c r="BB3" s="93"/>
+      <c r="BC3" s="93"/>
+      <c r="BD3" s="93"/>
+      <c r="BE3" s="93"/>
+      <c r="BF3" s="93"/>
+      <c r="BG3" s="93"/>
+      <c r="BH3" s="93"/>
+      <c r="BI3" s="93"/>
+      <c r="BJ3" s="93"/>
+      <c r="BK3" s="93"/>
+      <c r="BL3" s="93"/>
       <c r="BM3" s="43"/>
     </row>
     <row r="4" spans="1:66" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1684,17 +1690,17 @@
       <c r="C4" s="42"/>
       <c r="D4" s="42"/>
       <c r="E4" s="63"/>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="93"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="101"/>
       <c r="O4" s="143" t="s">
         <v>2</v>
       </c>
@@ -1779,15 +1785,15 @@
       <c r="C5" s="42"/>
       <c r="D5" s="42"/>
       <c r="E5" s="63"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="95"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="95"/>
-      <c r="N5" s="96"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="104"/>
       <c r="O5" s="146"/>
       <c r="P5" s="147"/>
       <c r="Q5" s="148"/>
@@ -2012,9 +2018,9 @@
     </row>
     <row r="7" spans="1:66" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="134"/>
-      <c r="B7" s="107"/>
-      <c r="C7" s="107"/>
-      <c r="D7" s="107"/>
+      <c r="B7" s="93"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
       <c r="E7" s="135"/>
       <c r="F7" s="139"/>
       <c r="G7" s="140"/>
@@ -2088,17 +2094,17 @@
       <c r="C8" s="45"/>
       <c r="D8" s="45"/>
       <c r="E8" s="46"/>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="86"/>
-      <c r="L8" s="86"/>
-      <c r="M8" s="86"/>
-      <c r="N8" s="87"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="97"/>
       <c r="O8" s="53">
         <v>0.5</v>
       </c>
@@ -2164,15 +2170,15 @@
       <c r="C9" s="48"/>
       <c r="D9" s="48"/>
       <c r="E9" s="49"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="89"/>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="89"/>
-      <c r="M9" s="89"/>
-      <c r="N9" s="90"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="83"/>
       <c r="O9" s="56"/>
       <c r="P9" s="57"/>
       <c r="Q9" s="58"/>
@@ -2234,17 +2240,17 @@
       <c r="C10" s="48"/>
       <c r="D10" s="48"/>
       <c r="E10" s="49"/>
-      <c r="F10" s="88" t="s">
+      <c r="F10" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="90"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="83"/>
       <c r="O10" s="53">
         <v>2</v>
       </c>
@@ -2312,15 +2318,15 @@
       <c r="C11" s="48"/>
       <c r="D11" s="48"/>
       <c r="E11" s="49"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="89"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="89"/>
-      <c r="L11" s="89"/>
-      <c r="M11" s="89"/>
-      <c r="N11" s="90"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="83"/>
       <c r="O11" s="56"/>
       <c r="P11" s="57"/>
       <c r="Q11" s="58"/>
@@ -2384,17 +2390,17 @@
       <c r="C12" s="48"/>
       <c r="D12" s="48"/>
       <c r="E12" s="49"/>
-      <c r="F12" s="89" t="s">
+      <c r="F12" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="89"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="89"/>
-      <c r="L12" s="89"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
       <c r="O12" s="53">
         <v>1</v>
       </c>
@@ -2460,15 +2466,15 @@
       <c r="C13" s="48"/>
       <c r="D13" s="48"/>
       <c r="E13" s="49"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="82"/>
+      <c r="L13" s="82"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
       <c r="O13" s="56"/>
       <c r="P13" s="57"/>
       <c r="Q13" s="58"/>
@@ -2530,17 +2536,17 @@
       <c r="C14" s="48"/>
       <c r="D14" s="48"/>
       <c r="E14" s="49"/>
-      <c r="F14" s="89" t="s">
+      <c r="F14" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="89"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="89"/>
-      <c r="N14" s="90"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="83"/>
       <c r="O14" s="53">
         <v>0.5</v>
       </c>
@@ -2606,15 +2612,15 @@
       <c r="C15" s="51"/>
       <c r="D15" s="51"/>
       <c r="E15" s="52"/>
-      <c r="F15" s="104"/>
-      <c r="G15" s="104"/>
-      <c r="H15" s="104"/>
-      <c r="I15" s="104"/>
-      <c r="J15" s="104"/>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="105"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="84"/>
+      <c r="N15" s="85"/>
       <c r="O15" s="56"/>
       <c r="P15" s="57"/>
       <c r="Q15" s="58"/>
@@ -3272,17 +3278,17 @@
       <c r="C24" s="45"/>
       <c r="D24" s="45"/>
       <c r="E24" s="46"/>
-      <c r="F24" s="100" t="s">
+      <c r="F24" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="100"/>
-      <c r="H24" s="100"/>
-      <c r="I24" s="100"/>
-      <c r="J24" s="100"/>
-      <c r="K24" s="100"/>
-      <c r="L24" s="100"/>
-      <c r="M24" s="100"/>
-      <c r="N24" s="101"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="105"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="105"/>
+      <c r="N24" s="106"/>
       <c r="O24" s="53">
         <v>1</v>
       </c>
@@ -3350,15 +3356,15 @@
       <c r="C25" s="51"/>
       <c r="D25" s="51"/>
       <c r="E25" s="52"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="102"/>
-      <c r="H25" s="102"/>
-      <c r="I25" s="102"/>
-      <c r="J25" s="102"/>
-      <c r="K25" s="102"/>
-      <c r="L25" s="102"/>
-      <c r="M25" s="102"/>
-      <c r="N25" s="103"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="107"/>
+      <c r="H25" s="107"/>
+      <c r="I25" s="107"/>
+      <c r="J25" s="107"/>
+      <c r="K25" s="107"/>
+      <c r="L25" s="107"/>
+      <c r="M25" s="107"/>
+      <c r="N25" s="108"/>
       <c r="O25" s="56"/>
       <c r="P25" s="57"/>
       <c r="Q25" s="58"/>
@@ -3422,17 +3428,17 @@
       <c r="C26" s="45"/>
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
-      <c r="F26" s="74" t="s">
+      <c r="F26" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="75"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="75"/>
-      <c r="K26" s="75"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="75"/>
-      <c r="N26" s="75"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="81"/>
+      <c r="J26" s="81"/>
+      <c r="K26" s="81"/>
+      <c r="L26" s="81"/>
+      <c r="M26" s="81"/>
+      <c r="N26" s="81"/>
       <c r="O26" s="53">
         <v>0.5</v>
       </c>
@@ -3498,15 +3504,15 @@
       <c r="C27" s="48"/>
       <c r="D27" s="48"/>
       <c r="E27" s="49"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
-      <c r="M27" s="75"/>
-      <c r="N27" s="75"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="81"/>
+      <c r="J27" s="81"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="81"/>
+      <c r="N27" s="81"/>
       <c r="O27" s="56"/>
       <c r="P27" s="57"/>
       <c r="Q27" s="58"/>
@@ -3568,17 +3574,17 @@
       <c r="C28" s="48"/>
       <c r="D28" s="48"/>
       <c r="E28" s="49"/>
-      <c r="F28" s="74" t="s">
+      <c r="F28" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="75"/>
-      <c r="K28" s="75"/>
-      <c r="L28" s="75"/>
-      <c r="M28" s="75"/>
-      <c r="N28" s="75"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="81"/>
+      <c r="L28" s="81"/>
+      <c r="M28" s="81"/>
+      <c r="N28" s="81"/>
       <c r="O28" s="53">
         <v>1</v>
       </c>
@@ -3644,15 +3650,15 @@
       <c r="C29" s="48"/>
       <c r="D29" s="48"/>
       <c r="E29" s="49"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="75"/>
-      <c r="N29" s="75"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="81"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="81"/>
+      <c r="N29" s="81"/>
       <c r="O29" s="56"/>
       <c r="P29" s="57"/>
       <c r="Q29" s="58"/>
@@ -3714,24 +3720,24 @@
       <c r="C30" s="48"/>
       <c r="D30" s="48"/>
       <c r="E30" s="49"/>
-      <c r="F30" s="74" t="s">
+      <c r="F30" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="75"/>
-      <c r="L30" s="75"/>
-      <c r="M30" s="75"/>
-      <c r="N30" s="75"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="81"/>
+      <c r="M30" s="81"/>
+      <c r="N30" s="81"/>
       <c r="O30" s="53">
         <v>4</v>
       </c>
       <c r="P30" s="54"/>
       <c r="Q30" s="55"/>
       <c r="R30" s="53">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="S30" s="54"/>
       <c r="T30" s="55"/>
@@ -3792,15 +3798,15 @@
       <c r="C31" s="48"/>
       <c r="D31" s="48"/>
       <c r="E31" s="49"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="75"/>
-      <c r="L31" s="75"/>
-      <c r="M31" s="75"/>
-      <c r="N31" s="75"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="81"/>
+      <c r="J31" s="81"/>
+      <c r="K31" s="81"/>
+      <c r="L31" s="81"/>
+      <c r="M31" s="81"/>
+      <c r="N31" s="81"/>
       <c r="O31" s="56"/>
       <c r="P31" s="57"/>
       <c r="Q31" s="58"/>
@@ -3831,8 +3837,10 @@
       </c>
       <c r="AK31" s="151"/>
       <c r="AL31" s="152"/>
-      <c r="AM31" s="7"/>
-      <c r="AN31" s="16"/>
+      <c r="AM31" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="AN31" s="156"/>
       <c r="AO31" s="8"/>
       <c r="AP31" s="8"/>
       <c r="AQ31" s="7"/>
@@ -3866,24 +3874,24 @@
       <c r="C32" s="48"/>
       <c r="D32" s="48"/>
       <c r="E32" s="49"/>
-      <c r="F32" s="74" t="s">
+      <c r="F32" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="75"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="75"/>
-      <c r="L32" s="75"/>
-      <c r="M32" s="75"/>
-      <c r="N32" s="75"/>
+      <c r="G32" s="81"/>
+      <c r="H32" s="81"/>
+      <c r="I32" s="81"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="81"/>
+      <c r="L32" s="81"/>
+      <c r="M32" s="81"/>
+      <c r="N32" s="81"/>
       <c r="O32" s="53">
         <v>4</v>
       </c>
       <c r="P32" s="54"/>
       <c r="Q32" s="55"/>
       <c r="R32" s="53">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="S32" s="54"/>
       <c r="T32" s="55"/>
@@ -3946,15 +3954,15 @@
       <c r="C33" s="48"/>
       <c r="D33" s="48"/>
       <c r="E33" s="49"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="75"/>
-      <c r="L33" s="75"/>
-      <c r="M33" s="75"/>
-      <c r="N33" s="75"/>
+      <c r="F33" s="81"/>
+      <c r="G33" s="81"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="81"/>
+      <c r="J33" s="81"/>
+      <c r="K33" s="81"/>
+      <c r="L33" s="81"/>
+      <c r="M33" s="81"/>
+      <c r="N33" s="81"/>
       <c r="O33" s="56"/>
       <c r="P33" s="57"/>
       <c r="Q33" s="58"/>
@@ -3981,7 +3989,9 @@
       <c r="AJ33" s="16"/>
       <c r="AK33" s="151"/>
       <c r="AL33" s="152"/>
-      <c r="AM33" s="7"/>
+      <c r="AM33" s="40">
+        <v>1.5</v>
+      </c>
       <c r="AN33" s="16"/>
       <c r="AO33" s="8"/>
       <c r="AP33" s="8"/>
@@ -4016,23 +4026,25 @@
       <c r="C34" s="48"/>
       <c r="D34" s="48"/>
       <c r="E34" s="49"/>
-      <c r="F34" s="74" t="s">
+      <c r="F34" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="75"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="75"/>
-      <c r="M34" s="75"/>
-      <c r="N34" s="75"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="81"/>
+      <c r="L34" s="81"/>
+      <c r="M34" s="81"/>
+      <c r="N34" s="81"/>
       <c r="O34" s="53">
         <v>3</v>
       </c>
       <c r="P34" s="54"/>
       <c r="Q34" s="55"/>
-      <c r="R34" s="53"/>
+      <c r="R34" s="53">
+        <v>1.5</v>
+      </c>
       <c r="S34" s="54"/>
       <c r="T34" s="55"/>
       <c r="U34" s="8"/>
@@ -4092,15 +4104,15 @@
       <c r="C35" s="48"/>
       <c r="D35" s="48"/>
       <c r="E35" s="49"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="75"/>
-      <c r="J35" s="75"/>
-      <c r="K35" s="75"/>
-      <c r="L35" s="75"/>
-      <c r="M35" s="75"/>
-      <c r="N35" s="75"/>
+      <c r="F35" s="81"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="81"/>
+      <c r="L35" s="81"/>
+      <c r="M35" s="81"/>
+      <c r="N35" s="81"/>
       <c r="O35" s="56"/>
       <c r="P35" s="57"/>
       <c r="Q35" s="58"/>
@@ -4126,9 +4138,10 @@
       <c r="AK35" s="151"/>
       <c r="AL35" s="152"/>
       <c r="AM35" s="7"/>
-      <c r="AN35" s="16"/>
+      <c r="AN35" s="38">
+        <v>1.5</v>
+      </c>
       <c r="AO35" s="8"/>
-      <c r="AP35" s="8"/>
       <c r="AQ35" s="7"/>
       <c r="AR35" s="16"/>
       <c r="AS35" s="7"/>
@@ -4160,17 +4173,17 @@
       <c r="C36" s="48"/>
       <c r="D36" s="48"/>
       <c r="E36" s="49"/>
-      <c r="F36" s="74" t="s">
+      <c r="F36" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="G36" s="75"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="75"/>
-      <c r="J36" s="75"/>
-      <c r="K36" s="75"/>
-      <c r="L36" s="75"/>
-      <c r="M36" s="75"/>
-      <c r="N36" s="75"/>
+      <c r="G36" s="81"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="81"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="81"/>
+      <c r="L36" s="81"/>
+      <c r="M36" s="81"/>
+      <c r="N36" s="81"/>
       <c r="O36" s="53">
         <v>3</v>
       </c>
@@ -4236,15 +4249,15 @@
       <c r="C37" s="48"/>
       <c r="D37" s="48"/>
       <c r="E37" s="49"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="75"/>
-      <c r="J37" s="75"/>
-      <c r="K37" s="75"/>
-      <c r="L37" s="75"/>
-      <c r="M37" s="75"/>
-      <c r="N37" s="75"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="81"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="81"/>
+      <c r="L37" s="81"/>
+      <c r="M37" s="81"/>
+      <c r="N37" s="81"/>
       <c r="O37" s="56"/>
       <c r="P37" s="57"/>
       <c r="Q37" s="58"/>
@@ -4304,17 +4317,17 @@
       <c r="C38" s="48"/>
       <c r="D38" s="48"/>
       <c r="E38" s="49"/>
-      <c r="F38" s="74" t="s">
+      <c r="F38" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="G38" s="75"/>
-      <c r="H38" s="75"/>
-      <c r="I38" s="75"/>
-      <c r="J38" s="75"/>
-      <c r="K38" s="75"/>
-      <c r="L38" s="75"/>
-      <c r="M38" s="75"/>
-      <c r="N38" s="75"/>
+      <c r="G38" s="81"/>
+      <c r="H38" s="81"/>
+      <c r="I38" s="81"/>
+      <c r="J38" s="81"/>
+      <c r="K38" s="81"/>
+      <c r="L38" s="81"/>
+      <c r="M38" s="81"/>
+      <c r="N38" s="81"/>
       <c r="O38" s="53">
         <v>3</v>
       </c>
@@ -4382,15 +4395,15 @@
       <c r="C39" s="48"/>
       <c r="D39" s="48"/>
       <c r="E39" s="49"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="75"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="75"/>
-      <c r="J39" s="75"/>
-      <c r="K39" s="75"/>
-      <c r="L39" s="75"/>
-      <c r="M39" s="75"/>
-      <c r="N39" s="75"/>
+      <c r="F39" s="81"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="81"/>
+      <c r="J39" s="81"/>
+      <c r="K39" s="81"/>
+      <c r="L39" s="81"/>
+      <c r="M39" s="81"/>
+      <c r="N39" s="81"/>
       <c r="O39" s="56"/>
       <c r="P39" s="57"/>
       <c r="Q39" s="58"/>
@@ -4598,17 +4611,17 @@
       <c r="C42" s="45"/>
       <c r="D42" s="45"/>
       <c r="E42" s="46"/>
-      <c r="F42" s="76" t="s">
+      <c r="F42" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="G42" s="77"/>
-      <c r="H42" s="77"/>
-      <c r="I42" s="77"/>
-      <c r="J42" s="77"/>
-      <c r="K42" s="77"/>
-      <c r="L42" s="77"/>
-      <c r="M42" s="77"/>
-      <c r="N42" s="78"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="72"/>
+      <c r="N42" s="73"/>
       <c r="O42" s="53">
         <v>2.5</v>
       </c>
@@ -4674,15 +4687,15 @@
       <c r="C43" s="48"/>
       <c r="D43" s="48"/>
       <c r="E43" s="49"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="80"/>
-      <c r="H43" s="80"/>
-      <c r="I43" s="80"/>
-      <c r="J43" s="80"/>
-      <c r="K43" s="80"/>
-      <c r="L43" s="80"/>
-      <c r="M43" s="80"/>
-      <c r="N43" s="81"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="75"/>
+      <c r="J43" s="75"/>
+      <c r="K43" s="75"/>
+      <c r="L43" s="75"/>
+      <c r="M43" s="75"/>
+      <c r="N43" s="76"/>
       <c r="O43" s="56"/>
       <c r="P43" s="57"/>
       <c r="Q43" s="58"/>
@@ -4742,17 +4755,17 @@
       <c r="C44" s="48"/>
       <c r="D44" s="48"/>
       <c r="E44" s="49"/>
-      <c r="F44" s="79" t="s">
+      <c r="F44" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="G44" s="80"/>
-      <c r="H44" s="80"/>
-      <c r="I44" s="80"/>
-      <c r="J44" s="80"/>
-      <c r="K44" s="80"/>
-      <c r="L44" s="80"/>
-      <c r="M44" s="80"/>
-      <c r="N44" s="81"/>
+      <c r="G44" s="75"/>
+      <c r="H44" s="75"/>
+      <c r="I44" s="75"/>
+      <c r="J44" s="75"/>
+      <c r="K44" s="75"/>
+      <c r="L44" s="75"/>
+      <c r="M44" s="75"/>
+      <c r="N44" s="76"/>
       <c r="O44" s="53">
         <v>3</v>
       </c>
@@ -5176,17 +5189,17 @@
       <c r="C50" s="45"/>
       <c r="D50" s="45"/>
       <c r="E50" s="46"/>
-      <c r="F50" s="97" t="s">
+      <c r="F50" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="G50" s="98"/>
-      <c r="H50" s="98"/>
-      <c r="I50" s="98"/>
-      <c r="J50" s="98"/>
-      <c r="K50" s="98"/>
-      <c r="L50" s="98"/>
-      <c r="M50" s="98"/>
-      <c r="N50" s="99"/>
+      <c r="G50" s="78"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="78"/>
+      <c r="L50" s="78"/>
+      <c r="M50" s="78"/>
+      <c r="N50" s="79"/>
       <c r="O50" s="53">
         <v>1.5</v>
       </c>
@@ -6239,7 +6252,7 @@
       <c r="P64" s="54"/>
       <c r="Q64" s="55"/>
       <c r="R64" s="53">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="S64" s="54"/>
       <c r="T64" s="55"/>
@@ -6360,7 +6373,9 @@
       <c r="AK65" s="151"/>
       <c r="AL65" s="152"/>
       <c r="AM65" s="7"/>
-      <c r="AN65" s="16"/>
+      <c r="AN65" s="38">
+        <v>0.5</v>
+      </c>
       <c r="AO65" s="8"/>
       <c r="AP65" s="8"/>
       <c r="AQ65" s="7"/>
@@ -6618,15 +6633,15 @@
       <c r="C69" s="51"/>
       <c r="D69" s="51"/>
       <c r="E69" s="52"/>
-      <c r="F69" s="71"/>
-      <c r="G69" s="72"/>
-      <c r="H69" s="72"/>
-      <c r="I69" s="72"/>
-      <c r="J69" s="72"/>
-      <c r="K69" s="72"/>
-      <c r="L69" s="72"/>
-      <c r="M69" s="72"/>
-      <c r="N69" s="73"/>
+      <c r="F69" s="89"/>
+      <c r="G69" s="90"/>
+      <c r="H69" s="90"/>
+      <c r="I69" s="90"/>
+      <c r="J69" s="90"/>
+      <c r="K69" s="90"/>
+      <c r="L69" s="90"/>
+      <c r="M69" s="90"/>
+      <c r="N69" s="91"/>
       <c r="O69" s="56"/>
       <c r="P69" s="57"/>
       <c r="Q69" s="58"/>
@@ -6652,7 +6667,7 @@
       <c r="AK69" s="153"/>
       <c r="AL69" s="154"/>
       <c r="AM69" s="2"/>
-      <c r="AN69" s="17"/>
+      <c r="AN69" s="157"/>
       <c r="AO69" s="14"/>
       <c r="AP69" s="14"/>
       <c r="AQ69" s="2"/>
@@ -6703,7 +6718,7 @@
       <c r="Q70" s="49"/>
       <c r="R70" s="44">
         <f>SUM(R6:T69)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="S70" s="45"/>
       <c r="T70" s="46"/>
@@ -6845,16 +6860,16 @@
       <c r="L72" s="42"/>
       <c r="M72" s="42"/>
       <c r="N72" s="63"/>
-      <c r="O72" s="82" t="s">
+      <c r="O72" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="P72" s="83"/>
-      <c r="Q72" s="84"/>
-      <c r="R72" s="82" t="s">
+      <c r="P72" s="87"/>
+      <c r="Q72" s="88"/>
+      <c r="R72" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="S72" s="83"/>
-      <c r="T72" s="84"/>
+      <c r="S72" s="87"/>
+      <c r="T72" s="88"/>
       <c r="U72" s="64"/>
       <c r="V72" s="65"/>
       <c r="W72" s="65"/>
@@ -7887,6 +7902,7 @@
     <mergeCell ref="R48:T49"/>
     <mergeCell ref="R40:T41"/>
     <mergeCell ref="R46:T47"/>
+    <mergeCell ref="O12:Q13"/>
     <mergeCell ref="R54:T55"/>
     <mergeCell ref="R56:T57"/>
     <mergeCell ref="F60:N61"/>
@@ -7911,7 +7927,6 @@
     <mergeCell ref="O22:Q23"/>
     <mergeCell ref="F24:N25"/>
     <mergeCell ref="F12:N13"/>
-    <mergeCell ref="O12:Q13"/>
     <mergeCell ref="R12:T13"/>
     <mergeCell ref="O14:Q15"/>
     <mergeCell ref="R14:T15"/>

</xml_diff>